<commit_message>
UC9a test Scenario in progress v2
</commit_message>
<xml_diff>
--- a/Testes/UC9a_Test_Scenario.xlsx
+++ b/Testes/UC9a_Test_Scenario.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23716"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB3F38EE-205D-4E61-A29F-D1D7F0FEE778}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{70FB93CD-CB51-41C7-880E-D90ED048B58B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
   <si>
     <t>Project Name</t>
   </si>
@@ -76,22 +76,91 @@
     <t>TC_Seriação_004</t>
   </si>
   <si>
+    <t>TC_Seriação_005</t>
+  </si>
+  <si>
+    <t>TC_Seriação_006</t>
+  </si>
+  <si>
+    <t>TC_Seriação_007</t>
+  </si>
+  <si>
+    <t>TC_Seriação_008</t>
+  </si>
+  <si>
     <t>Test Case Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Colaborador da </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valid User
-Invalid Password </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invalid User
-Valid Password </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invalid User
-Invalid Password </t>
+    <t>1.Colaborador da organização registado.
+2.Tarefa publicada.
+3.Periodo de candidaturas terminado.
+4.Periodo de seriação iniciado.
+5.Candidaturas à tarefa ainda não seriadas.
+6.Tarefa ainda não adjudicada.
+7.Existe pelo menos uma candidatura à tarefa.</t>
+  </si>
+  <si>
+    <t>1.Colaborador da organização registado.
+2.Tarefa publicada.
+3.Periodo de candidaturas terminado.
+4.Periodo de seriação iniciado.
+5.Candidaturas à tarefa ainda não seriadas.
+6.Tarefa ainda não adjudicada.
+7.Não existem candidaturas à tarefa</t>
+  </si>
+  <si>
+    <t>1.Colaborador da organização registado.
+2.Tarefa publicada.
+3.Periodo de candidaturas terminado.
+4.Periodo de seriação iniciado.
+5.Candidaturas à tarefa ainda não seriadas.
+6.Tarefa já adjudicada
+7.Existe pelo menos uma candidatura à tarefa.</t>
+  </si>
+  <si>
+    <t>1.Colaborador da organização registado.
+2.Tarefa publicada.
+3.Periodo de candidaturas terminado.
+4.Periodo de seriação iniciado.
+5.Candidaturas à tarefa já seriadas.
+6.Tarefa ainda não adjudicada.
+7.Existe pelo menos uma candidatura à tarefa.</t>
+  </si>
+  <si>
+    <t>1.Colaborador da organização registado.
+2.Tarefa publicada.
+3.Periodo de candidaturas terminado.
+4.Periodo de seriação ainda não iniciado.
+5.Candidaturas à tarefa ainda não seriadas.
+6.Tarefa ainda não adjudicada.
+7.Existe pelo menos uma candidatura à tarefa.</t>
+  </si>
+  <si>
+    <t>1.Colaborador da organização registado.
+2.Tarefa publicada.
+3.Periodo de candidaturas a decorrer.
+4.Periodo de seriação iniciado.
+5.Candidaturas à tarefa ainda não seriadas.
+6.Tarefa ainda não adjudicada.
+7.Existe pelo menos uma candidatura à tarefa.</t>
+  </si>
+  <si>
+    <t>1.Colaborador da organização registado.
+2.Tarefa não publicada.
+3.Periodo de candidaturas terminado.
+4.Periodo de seriação iniciado.
+5.Candidaturas à tarefa ainda não seriadas.
+6.Tarefa ainda não adjudicada.
+7.Existe pelo menos uma candidatura à tarefa.</t>
+  </si>
+  <si>
+    <t>1.Colaborador da organização não está registado.
+2.Tarefa publicada.
+3.Periodo de candidaturas terminado.
+4.Periodo de seriação iniciado.
+5.Candidaturas à tarefa ainda não seriadas.
+6.Tarefa ainda não adjudicada.
+7.Existe pelo menos uma candidatura à tarefa.</t>
   </si>
   <si>
     <t>Test Case Steps</t>
@@ -131,19 +200,52 @@
     <t>Post Conditions</t>
   </si>
   <si>
-    <t>The user should be able to see the homepage</t>
-  </si>
-  <si>
-    <t>Error message "invalid user or password"</t>
+    <t>Tarefas seriadas de acordo com o regime pré-estabelecido</t>
+  </si>
+  <si>
+    <t>Error message "Não existem candidaturas para esta tarefa"</t>
+  </si>
+  <si>
+    <t>Error message "Esta tarefa já foi adjudicada"</t>
+  </si>
+  <si>
+    <t>Error message "As candidaturas para esta tarefa já foram seriadas"</t>
+  </si>
+  <si>
+    <t>Error message "Período de seriação ainda não iniciou."</t>
+  </si>
+  <si>
+    <t>Error message "Período de candidaturas para esta tarefa ainda não terminou."</t>
+  </si>
+  <si>
+    <t>Error message "Esta tarefa ainda não foi publicada"</t>
+  </si>
+  <si>
+    <t>Error message "Este colaborador não está registado."</t>
   </si>
   <si>
     <t>Expected Result</t>
   </si>
   <si>
-    <t>Successful login</t>
-  </si>
-  <si>
-    <t>Popup Message: Invalid username or password</t>
+    <t>Seriação efetuada com sucesso</t>
+  </si>
+  <si>
+    <t>Popup Message: Não existem candidaturas para esta tarefa</t>
+  </si>
+  <si>
+    <t>Popup Message: Esta tarefa já foi adjudicada</t>
+  </si>
+  <si>
+    <t>Popup Message: As candidaturas para esta tarefa já foram seriadas</t>
+  </si>
+  <si>
+    <t>Popup Message: Período de seriação ainda não iniciou.</t>
+  </si>
+  <si>
+    <t>Popup Message: Esta tarefa ainda não foi publicada.</t>
+  </si>
+  <si>
+    <t>Popup Message: Este colaborador não está registado.</t>
   </si>
   <si>
     <t>Actual Result</t>
@@ -187,7 +289,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,6 +300,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE4D6"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -229,13 +343,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -621,59 +750,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="23.75"/>
     <col min="2" max="2" width="45" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.875" customWidth="1"/>
-    <col min="4" max="4" width="36" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="4" max="4" width="33.75" customWidth="1"/>
     <col min="5" max="5" width="34.625" customWidth="1"/>
-    <col min="6" max="1025" width="10.875"/>
+    <col min="6" max="6" width="33.5" customWidth="1"/>
+    <col min="7" max="7" width="33.25" customWidth="1"/>
+    <col min="8" max="8" width="36" customWidth="1"/>
+    <col min="9" max="9" width="30.25" customWidth="1"/>
+    <col min="10" max="1025" width="10.875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6"/>
     </row>
-    <row r="8" spans="1:5" ht="15.75">
+    <row r="8" spans="1:9" ht="15.75">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -689,8 +822,20 @@
       <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="31.5">
+      <c r="F8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="63">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -706,8 +851,20 @@
       <c r="E9" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75">
+      <c r="F9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="31.5">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -723,146 +880,227 @@
       <c r="E10" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="31.5">
+      <c r="F10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="177" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="204.75">
-      <c r="A12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75">
+        <v>23</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="7" customFormat="1" ht="305.25" customHeight="1">
+      <c r="A12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75">
       <c r="A13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="31.5">
+        <v>30</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="63">
       <c r="A14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="31.5">
+        <v>31</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="47.25">
       <c r="A15" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="31.5">
+        <v>40</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="31.5">
       <c r="A16" s="2" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75">
+        <v>49</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75">
       <c r="A17" s="2" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="B17"/>
     </row>
-    <row r="18" spans="1:5" ht="15.75">
+    <row r="18" spans="1:9" ht="15.75">
       <c r="A18" s="2" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>56</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" t="s">
+        <v>56</v>
+      </c>
+      <c r="I18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75">
       <c r="A19" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>57</v>
+      </c>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75">
       <c r="A20" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>58</v>
+      </c>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" ht="15.75">
       <c r="A21" s="2" t="s">
-        <v>40</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
UC9a test Scenario in progress v3
</commit_message>
<xml_diff>
--- a/Testes/UC9a_Test_Scenario.xlsx
+++ b/Testes/UC9a_Test_Scenario.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23716"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70FB93CD-CB51-41C7-880E-D90ED048B58B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C535E03-AE61-46F9-AFF8-13A31A086B8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="61">
   <si>
     <t>Project Name</t>
   </si>
@@ -181,20 +181,26 @@
     <t>Test Data</t>
   </si>
   <si>
+    <t xml:space="preserve">1.Colaborador da organização registado.
+2.Tarefa publicada.
+3.Período de candidaturas terminou a 8-01-2021.
+4.Período de seriação iniciou a 10-01-2021 e termina a </t>
+  </si>
+  <si>
+    <t>username: a@b.pt
+password: xxxx</t>
+  </si>
+  <si>
+    <t>username: a@b.
+password: 1234</t>
+  </si>
+  <si>
+    <t>username: a@b.
+password: xxxx</t>
+  </si>
+  <si>
     <t>username: a@b.pt
 password: 1234</t>
-  </si>
-  <si>
-    <t>username: a@b.pt
-password: xxxx</t>
-  </si>
-  <si>
-    <t>username: a@b.
-password: 1234</t>
-  </si>
-  <si>
-    <t>username: a@b.
-password: xxxx</t>
   </si>
   <si>
     <t>Post Conditions</t>
@@ -753,7 +759,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95"/>
@@ -971,7 +977,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="63">
+    <row r="14" spans="1:9" ht="78.75">
       <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
@@ -988,117 +994,117 @@
         <v>35</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="47.25">
       <c r="A15" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="31.5">
       <c r="A16" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75">
       <c r="A17" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B17"/>
     </row>
     <row r="18" spans="1:9" ht="15.75">
       <c r="A18" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75">
       <c r="A19" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:9" ht="15.75">
       <c r="A20" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:9" ht="15.75">
       <c r="A21" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F21" s="1"/>
     </row>

</xml_diff>

<commit_message>
Update UC9TS e inicio UC10TS
</commit_message>
<xml_diff>
--- a/Testes/UC9a_Test_Scenario.xlsx
+++ b/Testes/UC9a_Test_Scenario.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23716"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{701FCB1D-7137-45AB-9E17-CB046D3D2138}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F0F769C-1FD2-41A2-92D9-E5EE95FB914D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
     <t>Test Scenario ID</t>
   </si>
   <si>
-    <t>TS_9a</t>
+    <t>UC09a_TS_001</t>
   </si>
   <si>
     <t>Test Scenario Description</t>
@@ -64,28 +64,28 @@
     <t>Test Case ID</t>
   </si>
   <si>
-    <t>TC_Seriação_001</t>
-  </si>
-  <si>
-    <t>TC_Seriação_002</t>
-  </si>
-  <si>
-    <t>TC_Seriação_003</t>
-  </si>
-  <si>
-    <t>TC_Seriação_004</t>
-  </si>
-  <si>
-    <t>TC_Seriação_005</t>
-  </si>
-  <si>
-    <t>TC_Seriação_006</t>
-  </si>
-  <si>
-    <t>TC_Seriação_007</t>
-  </si>
-  <si>
-    <t>TC_Seriação_008</t>
+    <t>TC_Ser_001</t>
+  </si>
+  <si>
+    <t>TC_Ser_002</t>
+  </si>
+  <si>
+    <t>TC_Ser_003</t>
+  </si>
+  <si>
+    <t>TC_Ser_004</t>
+  </si>
+  <si>
+    <t>TC_Ser_005</t>
+  </si>
+  <si>
+    <t>TC_Ser_006</t>
+  </si>
+  <si>
+    <t>TC_Ser_007</t>
+  </si>
+  <si>
+    <t>TC_Ser_008</t>
   </si>
   <si>
     <t>Test Case Description</t>
@@ -393,21 +393,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -419,6 +410,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -805,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95"/>
@@ -917,7 +911,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="31.5">
+    <row r="10" spans="1:9" ht="15.75">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -946,61 +940,61 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="177" customHeight="1">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:9" s="6" customFormat="1" ht="177" customHeight="1">
+      <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="5" customFormat="1" ht="305.25" customHeight="1">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:9" s="6" customFormat="1" ht="305.25" customHeight="1">
+      <c r="A12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1008,48 +1002,48 @@
       <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="9" customFormat="1" ht="189">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:9" s="6" customFormat="1" ht="189">
+      <c r="A14" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="5" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>